<commit_message>
Continuing to examine effects of QRPs.
</commit_message>
<xml_diff>
--- a/tables/mastertable.xlsx
+++ b/tables/mastertable.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="pow_table" sheetId="6" r:id="rId1"/>
@@ -438,8 +438,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="O32" sqref="O32:P37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1172,7 +1172,7 @@
         <v>0.99399999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0</v>
       </c>
@@ -1228,7 +1228,7 @@
         <v>0.998</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0</v>
       </c>
@@ -1284,7 +1284,7 @@
         <v>0.997</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>0</v>
       </c>
@@ -1340,7 +1340,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>0.5</v>
       </c>
@@ -1396,7 +1396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>0.5</v>
       </c>
@@ -1452,7 +1452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>0.5</v>
       </c>
@@ -1508,7 +1508,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>0</v>
       </c>
@@ -1564,7 +1564,7 @@
         <v>0.88900000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>0</v>
       </c>
@@ -1620,7 +1620,7 @@
         <v>0.80400000000000005</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>0</v>
       </c>
@@ -1676,7 +1676,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>0.5</v>
       </c>
@@ -1732,7 +1732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>0.5</v>
       </c>
@@ -1788,7 +1788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>0.5</v>
       </c>
@@ -1844,7 +1844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>0</v>
       </c>
@@ -1900,15 +1900,15 @@
         <v>0.80200000000000005</v>
       </c>
     </row>
-    <row r="27" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="B27">
         <v>0</v>
       </c>
       <c r="C27" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D27" t="s">
         <v>0</v>
@@ -1920,16 +1920,16 @@
         <v>1</v>
       </c>
       <c r="G27">
-        <v>1</v>
+        <v>0.97148676171079396</v>
       </c>
       <c r="H27">
         <v>1</v>
       </c>
       <c r="I27">
-        <v>0.52700000000000002</v>
+        <v>0.11899999999999999</v>
       </c>
       <c r="J27">
-        <v>0.998</v>
+        <v>0.32600000000000001</v>
       </c>
       <c r="K27" t="s">
         <v>21</v>
@@ -1944,48 +1944,48 @@
         <v>21</v>
       </c>
       <c r="O27">
-        <v>0.94225721784776895</v>
+        <v>5.8020477815699703E-2</v>
       </c>
       <c r="P27">
-        <v>0.99688149688149696</v>
+        <v>0.115</v>
       </c>
       <c r="Q27">
-        <v>0.96199999999999997</v>
+        <v>0.94299999999999995</v>
       </c>
       <c r="R27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>0</v>
       </c>
       <c r="B28">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C28" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D28" t="s">
         <v>0</v>
       </c>
       <c r="E28">
-        <v>0.94599999999999995</v>
+        <v>1</v>
       </c>
       <c r="F28">
         <v>1</v>
       </c>
       <c r="G28">
-        <v>0.81039755351681997</v>
+        <v>0.98858921161825697</v>
       </c>
       <c r="H28">
         <v>1</v>
       </c>
       <c r="I28">
-        <v>0.20399999999999999</v>
+        <v>0.127</v>
       </c>
       <c r="J28">
-        <v>0.36799999999999999</v>
+        <v>0.45200000000000001</v>
       </c>
       <c r="K28" t="s">
         <v>21</v>
@@ -2000,21 +2000,21 @@
         <v>21</v>
       </c>
       <c r="O28">
-        <v>0.42116402116402102</v>
+        <v>2.95774647887324E-2</v>
       </c>
       <c r="P28">
-        <v>0.52300000000000002</v>
+        <v>0.112112112112112</v>
       </c>
       <c r="Q28">
-        <v>0.64100000000000001</v>
+        <v>0.94199999999999995</v>
       </c>
       <c r="R28">
-        <v>0.73899999999999999</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>0.73399999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="B29">
         <v>0.2</v>
@@ -2026,22 +2026,22 @@
         <v>0</v>
       </c>
       <c r="E29">
-        <v>1</v>
+        <v>0.94599999999999995</v>
       </c>
       <c r="F29">
         <v>1</v>
       </c>
       <c r="G29">
-        <v>1</v>
+        <v>0.81039755351681997</v>
       </c>
       <c r="H29">
         <v>1</v>
       </c>
       <c r="I29">
-        <v>0.42599999999999999</v>
+        <v>0.20399999999999999</v>
       </c>
       <c r="J29">
-        <v>0.97399999999999998</v>
+        <v>0.36799999999999999</v>
       </c>
       <c r="K29" t="s">
         <v>21</v>
@@ -2056,24 +2056,24 @@
         <v>21</v>
       </c>
       <c r="O29">
-        <v>0.89572192513368998</v>
+        <v>0.42116402116402102</v>
       </c>
       <c r="P29">
-        <v>0.98740818467995795</v>
+        <v>0.52300000000000002</v>
       </c>
       <c r="Q29">
-        <v>0.95699999999999996</v>
+        <v>0.64100000000000001</v>
       </c>
       <c r="R29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>0.73899999999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>0</v>
       </c>
       <c r="B30">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="C30" t="s">
         <v>1</v>
@@ -2082,22 +2082,22 @@
         <v>0</v>
       </c>
       <c r="E30">
-        <v>1</v>
+        <v>0.98499999999999999</v>
       </c>
       <c r="F30">
         <v>1</v>
       </c>
       <c r="G30">
-        <v>0.97148676171079396</v>
+        <v>0.88381742738589197</v>
       </c>
       <c r="H30">
         <v>1</v>
       </c>
       <c r="I30">
-        <v>0.11899999999999999</v>
+        <v>0.16900000000000001</v>
       </c>
       <c r="J30">
-        <v>0.32600000000000001</v>
+        <v>0.23100000000000001</v>
       </c>
       <c r="K30" t="s">
         <v>21</v>
@@ -2112,104 +2112,104 @@
         <v>21</v>
       </c>
       <c r="O30">
-        <v>5.8020477815699703E-2</v>
+        <v>0.12407680945347099</v>
       </c>
       <c r="P30">
-        <v>0.115</v>
+        <v>0.119119119119119</v>
       </c>
       <c r="Q30">
-        <v>0.94299999999999995</v>
+        <v>0.70899999999999996</v>
       </c>
       <c r="R30">
-        <v>0.63</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31">
+        <v>0</v>
+      </c>
+      <c r="B31">
+        <v>0.2</v>
+      </c>
+      <c r="C31" t="s">
+        <v>0</v>
+      </c>
+      <c r="D31" t="s">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0.99</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
+      <c r="G31">
+        <v>0.92394655704008199</v>
+      </c>
+      <c r="H31">
+        <v>1</v>
+      </c>
+      <c r="I31">
+        <v>0.159</v>
+      </c>
+      <c r="J31">
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="K31" t="s">
+        <v>21</v>
+      </c>
+      <c r="L31" t="s">
+        <v>21</v>
+      </c>
+      <c r="M31" t="s">
+        <v>21</v>
+      </c>
+      <c r="N31" t="s">
+        <v>21</v>
+      </c>
+      <c r="O31">
+        <v>5.6818181818181802E-2</v>
+      </c>
+      <c r="P31">
+        <v>0.13636363636363599</v>
+      </c>
+      <c r="Q31">
+        <v>0.70099999999999996</v>
+      </c>
+      <c r="R31">
+        <v>0.71399999999999997</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A32">
         <v>0.5</v>
       </c>
-      <c r="B31">
-        <v>0</v>
-      </c>
-      <c r="C31" t="s">
-        <v>1</v>
-      </c>
-      <c r="D31" t="s">
-        <v>0</v>
-      </c>
-      <c r="E31">
-        <v>1</v>
-      </c>
-      <c r="F31">
-        <v>1</v>
-      </c>
-      <c r="G31">
-        <v>1</v>
-      </c>
-      <c r="H31">
-        <v>1</v>
-      </c>
-      <c r="I31">
-        <v>0.52300000000000002</v>
-      </c>
-      <c r="J31">
-        <v>0.999</v>
-      </c>
-      <c r="K31" t="s">
-        <v>21</v>
-      </c>
-      <c r="L31" t="s">
-        <v>21</v>
-      </c>
-      <c r="M31" t="s">
-        <v>21</v>
-      </c>
-      <c r="N31" t="s">
-        <v>21</v>
-      </c>
-      <c r="O31">
-        <v>0.82882882882882902</v>
-      </c>
-      <c r="P31">
-        <v>0.97264957264957297</v>
-      </c>
-      <c r="Q31">
-        <v>0.93</v>
-      </c>
-      <c r="R31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>0</v>
-      </c>
       <c r="B32">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C32" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D32" t="s">
         <v>0</v>
       </c>
       <c r="E32">
-        <v>0.98499999999999999</v>
+        <v>1</v>
       </c>
       <c r="F32">
         <v>1</v>
       </c>
       <c r="G32">
-        <v>0.88381742738589197</v>
+        <v>1</v>
       </c>
       <c r="H32">
         <v>1</v>
       </c>
       <c r="I32">
-        <v>0.16900000000000001</v>
+        <v>0.52700000000000002</v>
       </c>
       <c r="J32">
-        <v>0.23100000000000001</v>
+        <v>0.998</v>
       </c>
       <c r="K32" t="s">
         <v>21</v>
@@ -2224,24 +2224,24 @@
         <v>21</v>
       </c>
       <c r="O32">
-        <v>0.12407680945347099</v>
+        <v>0.94225721784776895</v>
       </c>
       <c r="P32">
-        <v>0.119119119119119</v>
+        <v>0.99688149688149696</v>
       </c>
       <c r="Q32">
-        <v>0.70899999999999996</v>
+        <v>0.96199999999999997</v>
       </c>
       <c r="R32">
-        <v>0.72</v>
-      </c>
-    </row>
-    <row r="33" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>0.5</v>
       </c>
       <c r="B33">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C33" t="s">
         <v>1</v>
@@ -2262,10 +2262,10 @@
         <v>1</v>
       </c>
       <c r="I33">
-        <v>0.41099999999999998</v>
+        <v>0.52300000000000002</v>
       </c>
       <c r="J33">
-        <v>0.95899999999999996</v>
+        <v>0.999</v>
       </c>
       <c r="K33" t="s">
         <v>21</v>
@@ -2280,21 +2280,21 @@
         <v>21</v>
       </c>
       <c r="O33">
-        <v>0.72222222222222199</v>
+        <v>0.82882882882882902</v>
       </c>
       <c r="P33">
-        <v>0.77403846153846201</v>
+        <v>0.97264957264957297</v>
       </c>
       <c r="Q33">
-        <v>0.93100000000000005</v>
+        <v>0.93</v>
       </c>
       <c r="R33">
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -2312,16 +2312,16 @@
         <v>1</v>
       </c>
       <c r="G34">
-        <v>0.98858921161825697</v>
+        <v>1</v>
       </c>
       <c r="H34">
         <v>1</v>
       </c>
       <c r="I34">
-        <v>0.127</v>
+        <v>0.53800000000000003</v>
       </c>
       <c r="J34">
-        <v>0.45200000000000001</v>
+        <v>0.997</v>
       </c>
       <c r="K34" t="s">
         <v>21</v>
@@ -2336,27 +2336,27 @@
         <v>21</v>
       </c>
       <c r="O34">
-        <v>2.95774647887324E-2</v>
+        <v>0.72307692307692295</v>
       </c>
       <c r="P34">
-        <v>0.112112112112112</v>
+        <v>0.95049504950495001</v>
       </c>
       <c r="Q34">
-        <v>0.94199999999999995</v>
+        <v>0.90900000000000003</v>
       </c>
       <c r="R34">
-        <v>0.73399999999999999</v>
-      </c>
-    </row>
-    <row r="35" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>0.5</v>
       </c>
       <c r="B35">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="C35" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D35" t="s">
         <v>0</v>
@@ -2374,10 +2374,10 @@
         <v>1</v>
       </c>
       <c r="I35">
-        <v>0.53800000000000003</v>
+        <v>0.42599999999999999</v>
       </c>
       <c r="J35">
-        <v>0.997</v>
+        <v>0.97399999999999998</v>
       </c>
       <c r="K35" t="s">
         <v>21</v>
@@ -2392,48 +2392,48 @@
         <v>21</v>
       </c>
       <c r="O35">
-        <v>0.72307692307692295</v>
+        <v>0.89572192513368998</v>
       </c>
       <c r="P35">
-        <v>0.95049504950495001</v>
+        <v>0.98740818467995795</v>
       </c>
       <c r="Q35">
-        <v>0.90900000000000003</v>
+        <v>0.95699999999999996</v>
       </c>
       <c r="R35">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="B36">
         <v>0.2</v>
       </c>
       <c r="C36" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D36" t="s">
         <v>0</v>
       </c>
       <c r="E36">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="F36">
         <v>1</v>
       </c>
       <c r="G36">
-        <v>0.92394655704008199</v>
+        <v>1</v>
       </c>
       <c r="H36">
         <v>1</v>
       </c>
       <c r="I36">
-        <v>0.159</v>
+        <v>0.41099999999999998</v>
       </c>
       <c r="J36">
-        <v>0.23400000000000001</v>
+        <v>0.95899999999999996</v>
       </c>
       <c r="K36" t="s">
         <v>21</v>
@@ -2448,19 +2448,19 @@
         <v>21</v>
       </c>
       <c r="O36">
-        <v>5.6818181818181802E-2</v>
+        <v>0.72222222222222199</v>
       </c>
       <c r="P36">
-        <v>0.13636363636363599</v>
+        <v>0.77403846153846201</v>
       </c>
       <c r="Q36">
-        <v>0.70099999999999996</v>
+        <v>0.93100000000000005</v>
       </c>
       <c r="R36">
-        <v>0.71399999999999997</v>
-      </c>
-    </row>
-    <row r="37" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>0.5</v>
       </c>
@@ -2520,11 +2520,11 @@
   <autoFilter ref="A1:R37">
     <filterColumn colId="3">
       <filters>
-        <filter val="med"/>
+        <filter val="high"/>
       </filters>
     </filterColumn>
-    <sortState ref="A14:R25">
-      <sortCondition ref="B1:B37"/>
+    <sortState ref="A26:R37">
+      <sortCondition ref="A1:A37"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2533,11 +2533,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14:R16"/>
+    <sheetView topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="Q29" sqref="Q29:R31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2598,7 +2597,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2654,7 +2653,7 @@
         <v>-2.6247149302211599E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -2710,7 +2709,7 @@
         <v>1.5730301012316299E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -2766,7 +2765,7 @@
         <v>2.4668847003642101E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0.5</v>
       </c>
@@ -2822,7 +2821,7 @@
         <v>-3.3921038283148699E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0.5</v>
       </c>
@@ -2878,7 +2877,7 @@
         <v>5.9057063107764499E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0.5</v>
       </c>
@@ -2934,7 +2933,7 @@
         <v>6.6888463294340001E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0</v>
       </c>
@@ -2990,7 +2989,7 @@
         <v>2.0179915770247598E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0</v>
       </c>
@@ -3046,7 +3045,7 @@
         <v>9.7290222042860797E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0</v>
       </c>
@@ -3102,7 +3101,7 @@
         <v>1.7658931018360701E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0.5</v>
       </c>
@@ -3158,7 +3157,7 @@
         <v>-1.6958003373259301E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0.5</v>
       </c>
@@ -3214,7 +3213,7 @@
         <v>-2.5635488220210501E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0.5</v>
       </c>
@@ -3942,7 +3941,7 @@
         <v>3.93388086566544E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>0</v>
       </c>
@@ -3998,121 +3997,121 @@
         <v>0.24900819764410501</v>
       </c>
     </row>
-    <row r="27" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="B27">
         <v>0</v>
       </c>
       <c r="C27" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D27" t="s">
         <v>0</v>
       </c>
       <c r="E27">
-        <v>7.2327901603395903E-2</v>
+        <v>0.38110109817985099</v>
       </c>
       <c r="F27">
-        <v>6.2540204804639205E-2</v>
+        <v>0.36876735041951803</v>
       </c>
       <c r="G27">
-        <v>3.45237532918879E-2</v>
+        <v>0.31619398174309399</v>
       </c>
       <c r="H27">
-        <v>9.8354995492400694E-3</v>
+        <v>0.30357314141994801</v>
       </c>
       <c r="I27">
-        <v>-0.16090890977428601</v>
+        <v>-0.10022221479340999</v>
       </c>
       <c r="J27">
-        <v>-5.2070461542399298E-2</v>
+        <v>-8.4463626177271101E-2</v>
       </c>
       <c r="K27">
-        <v>-5.8090563603023504E-3</v>
+        <v>2.6693479276690898E-2</v>
       </c>
       <c r="L27">
-        <v>-1.6342926942888799E-3</v>
+        <v>1.4193809934437401E-3</v>
       </c>
       <c r="M27">
-        <v>-8.8271878362391996E-3</v>
+        <v>0.117466821844983</v>
       </c>
       <c r="N27">
-        <v>-5.0252144188589901E-3</v>
+        <v>4.5650754744611798E-2</v>
       </c>
       <c r="O27">
-        <v>-6.3656064581461202E-3</v>
+        <v>6.5591113419807903E-2</v>
       </c>
       <c r="P27">
-        <v>-7.3539454455828698E-3</v>
+        <v>4.8657492382922697E-2</v>
       </c>
       <c r="Q27">
-        <v>2.94466232041007E-2</v>
+        <v>0.35395244150796601</v>
       </c>
       <c r="R27">
-        <v>2.1978122218089601E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>0.22061049209722999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>0</v>
       </c>
       <c r="B28">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C28" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D28" t="s">
         <v>0</v>
       </c>
       <c r="E28">
-        <v>0.38606355877095899</v>
+        <v>0.40674837802394898</v>
       </c>
       <c r="F28">
-        <v>0.38968633418598603</v>
+        <v>0.39264510260292101</v>
       </c>
       <c r="G28">
-        <v>0.32053897239578999</v>
+        <v>0.34132538858477801</v>
       </c>
       <c r="H28">
-        <v>0.30157411321282102</v>
+        <v>0.324473156893754</v>
       </c>
       <c r="I28">
-        <v>6.7185879930762804E-2</v>
+        <v>-0.101174962269748</v>
       </c>
       <c r="J28">
-        <v>0.116219804850691</v>
+        <v>-8.9770109921996605E-2</v>
       </c>
       <c r="K28">
-        <v>0.25453721439188398</v>
+        <v>2.3336439450052E-2</v>
       </c>
       <c r="L28">
-        <v>0.26815162506760298</v>
+        <v>6.7646404324579095E-4</v>
       </c>
       <c r="M28">
-        <v>0.27808527670556399</v>
+        <v>0.122217159526473</v>
       </c>
       <c r="N28">
-        <v>0.26763064028926098</v>
+        <v>5.7214744458342702E-2</v>
       </c>
       <c r="O28">
-        <v>0.1584234178459</v>
+        <v>5.8811056025830102E-2</v>
       </c>
       <c r="P28">
-        <v>0.13030703340417901</v>
+        <v>6.2870829543728801E-2</v>
       </c>
       <c r="Q28">
-        <v>0.33387746120762801</v>
+        <v>0.37763293389554098</v>
       </c>
       <c r="R28">
-        <v>0.25241472564837403</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>0.22175060130858701</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="B29">
         <v>0.2</v>
@@ -4124,54 +4123,54 @@
         <v>0</v>
       </c>
       <c r="E29">
-        <v>0.13669432419510499</v>
+        <v>0.38606355877095899</v>
       </c>
       <c r="F29">
-        <v>0.133556422960978</v>
+        <v>0.38968633418598603</v>
       </c>
       <c r="G29">
-        <v>8.8034132684122093E-2</v>
+        <v>0.32053897239578999</v>
       </c>
       <c r="H29">
-        <v>4.76508951287926E-2</v>
+        <v>0.30157411321282102</v>
       </c>
       <c r="I29">
-        <v>-0.153740183381916</v>
+        <v>6.7185879930762804E-2</v>
       </c>
       <c r="J29">
-        <v>-1.74943103340085E-2</v>
+        <v>0.116219804850691</v>
       </c>
       <c r="K29">
-        <v>7.3984191122947504E-2</v>
+        <v>0.25453721439188398</v>
       </c>
       <c r="L29">
-        <v>8.2185218147474801E-2</v>
+        <v>0.26815162506760298</v>
       </c>
       <c r="M29">
-        <v>7.1212371225103793E-2</v>
+        <v>0.27808527670556399</v>
       </c>
       <c r="N29">
-        <v>7.6545987057850803E-2</v>
+        <v>0.26763064028926098</v>
       </c>
       <c r="O29">
-        <v>3.4300796276771697E-2</v>
+        <v>0.1584234178459</v>
       </c>
       <c r="P29">
-        <v>1.5125065550481801E-2</v>
+        <v>0.13030703340417901</v>
       </c>
       <c r="Q29">
-        <v>8.0583988135130805E-2</v>
+        <v>0.33387746120762801</v>
       </c>
       <c r="R29">
-        <v>7.7359228864058105E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>0.25241472564837403</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>0</v>
       </c>
       <c r="B30">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="C30" t="s">
         <v>1</v>
@@ -4180,166 +4179,166 @@
         <v>0</v>
       </c>
       <c r="E30">
-        <v>0.38110109817985099</v>
+        <v>0.41359250877494302</v>
       </c>
       <c r="F30">
-        <v>0.36876735041951803</v>
+        <v>0.41088790435258998</v>
       </c>
       <c r="G30">
-        <v>0.31619398174309399</v>
+        <v>0.34211793931465301</v>
       </c>
       <c r="H30">
-        <v>0.30357314141994801</v>
+        <v>0.32522776405655301</v>
       </c>
       <c r="I30">
-        <v>-0.10022221479340999</v>
+        <v>-1.0002772580623299E-2</v>
       </c>
       <c r="J30">
-        <v>-8.4463626177271101E-2</v>
+        <v>1.3024551528731E-2</v>
       </c>
       <c r="K30">
-        <v>2.6693479276690898E-2</v>
+        <v>0.121593045999389</v>
       </c>
       <c r="L30">
-        <v>1.4193809934437401E-3</v>
+        <v>9.0791207540051599E-2</v>
       </c>
       <c r="M30">
-        <v>0.117466821844983</v>
+        <v>0.18736983988974901</v>
       </c>
       <c r="N30">
-        <v>4.5650754744611798E-2</v>
+        <v>0.11350386914011899</v>
       </c>
       <c r="O30">
-        <v>6.5591113419807903E-2</v>
+        <v>6.3736202157348001E-2</v>
       </c>
       <c r="P30">
-        <v>4.8657492382922697E-2</v>
+        <v>3.1879913937056997E-2</v>
       </c>
       <c r="Q30">
-        <v>0.35395244150796601</v>
+        <v>0.35748540626689401</v>
       </c>
       <c r="R30">
-        <v>0.22061049209722999</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>0.245242867866654</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31">
+        <v>0</v>
+      </c>
+      <c r="B31">
+        <v>0.2</v>
+      </c>
+      <c r="C31" t="s">
+        <v>0</v>
+      </c>
+      <c r="D31" t="s">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0.42524918622058799</v>
+      </c>
+      <c r="F31">
+        <v>0.42003666060161199</v>
+      </c>
+      <c r="G31">
+        <v>0.35425757480871101</v>
+      </c>
+      <c r="H31">
+        <v>0.33314751577169399</v>
+      </c>
+      <c r="I31">
+        <v>-3.9451326042871201E-2</v>
+      </c>
+      <c r="J31">
+        <v>-2.4805310862793001E-2</v>
+      </c>
+      <c r="K31">
+        <v>8.8992982801883294E-2</v>
+      </c>
+      <c r="L31">
+        <v>5.0310883541125402E-2</v>
+      </c>
+      <c r="M31">
+        <v>0.173348026120906</v>
+      </c>
+      <c r="N31">
+        <v>8.6832566524164795E-2</v>
+      </c>
+      <c r="O31">
+        <v>2.22095365532517E-2</v>
+      </c>
+      <c r="P31">
+        <v>3.8506265655108597E-2</v>
+      </c>
+      <c r="Q31">
+        <v>0.36375473227316302</v>
+      </c>
+      <c r="R31">
+        <v>0.241231551750235</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A32">
         <v>0.5</v>
       </c>
-      <c r="B31">
-        <v>0</v>
-      </c>
-      <c r="C31" t="s">
-        <v>1</v>
-      </c>
-      <c r="D31" t="s">
-        <v>0</v>
-      </c>
-      <c r="E31">
-        <v>7.4715530266486502E-2</v>
-      </c>
-      <c r="F31">
-        <v>6.5349363699750307E-2</v>
-      </c>
-      <c r="G31">
-        <v>3.3294454087978799E-2</v>
-      </c>
-      <c r="H31">
-        <v>9.8342467429351592E-3</v>
-      </c>
-      <c r="I31">
-        <v>-0.17585108565133201</v>
-      </c>
-      <c r="J31">
-        <v>-5.8016905404943399E-2</v>
-      </c>
-      <c r="K31">
-        <v>-6.6195760861759406E-2</v>
-      </c>
-      <c r="L31">
-        <v>-4.9620274821055799E-2</v>
-      </c>
-      <c r="M31">
-        <v>-6.7308511921754896E-2</v>
-      </c>
-      <c r="N31">
-        <v>-5.3466620786926398E-2</v>
-      </c>
-      <c r="O31">
-        <v>-5.32256130875376E-2</v>
-      </c>
-      <c r="P31">
-        <v>-3.99429733484368E-2</v>
-      </c>
-      <c r="Q31">
-        <v>2.2024631149884601E-2</v>
-      </c>
-      <c r="R31">
-        <v>1.88576238273837E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>0</v>
-      </c>
       <c r="B32">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C32" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D32" t="s">
         <v>0</v>
       </c>
       <c r="E32">
-        <v>0.41359250877494302</v>
+        <v>7.2327901603395903E-2</v>
       </c>
       <c r="F32">
-        <v>0.41088790435258998</v>
+        <v>6.2540204804639205E-2</v>
       </c>
       <c r="G32">
-        <v>0.34211793931465301</v>
+        <v>3.45237532918879E-2</v>
       </c>
       <c r="H32">
-        <v>0.32522776405655301</v>
+        <v>9.8354995492400694E-3</v>
       </c>
       <c r="I32">
-        <v>-1.0002772580623299E-2</v>
+        <v>-0.16090890977428601</v>
       </c>
       <c r="J32">
-        <v>1.3024551528731E-2</v>
+        <v>-5.2070461542399298E-2</v>
       </c>
       <c r="K32">
-        <v>0.121593045999389</v>
+        <v>-5.8090563603023504E-3</v>
       </c>
       <c r="L32">
-        <v>9.0791207540051599E-2</v>
+        <v>-1.6342926942888799E-3</v>
       </c>
       <c r="M32">
-        <v>0.18736983988974901</v>
+        <v>-8.8271878362391996E-3</v>
       </c>
       <c r="N32">
-        <v>0.11350386914011899</v>
+        <v>-5.0252144188589901E-3</v>
       </c>
       <c r="O32">
-        <v>6.3736202157348001E-2</v>
+        <v>-6.3656064581461202E-3</v>
       </c>
       <c r="P32">
-        <v>3.1879913937056997E-2</v>
+        <v>-7.3539454455828698E-3</v>
       </c>
       <c r="Q32">
-        <v>0.35748540626689401</v>
+        <v>2.94466232041007E-2</v>
       </c>
       <c r="R32">
-        <v>0.245242867866654</v>
-      </c>
-    </row>
-    <row r="33" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>2.1978122218089601E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>0.5</v>
       </c>
       <c r="B33">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C33" t="s">
         <v>1</v>
@@ -4348,51 +4347,51 @@
         <v>0</v>
       </c>
       <c r="E33">
-        <v>0.12181965733904</v>
+        <v>7.4715530266486502E-2</v>
       </c>
       <c r="F33">
-        <v>0.115875322460899</v>
+        <v>6.5349363699750307E-2</v>
       </c>
       <c r="G33">
-        <v>7.3244517179751306E-2</v>
+        <v>3.3294454087978799E-2</v>
       </c>
       <c r="H33">
-        <v>3.0831589694546701E-2</v>
+        <v>9.8342467429351592E-3</v>
       </c>
       <c r="I33">
-        <v>-0.16859766473228599</v>
+        <v>-0.17585108565133201</v>
       </c>
       <c r="J33">
-        <v>-4.1722740165033301E-2</v>
+        <v>-5.8016905404943399E-2</v>
       </c>
       <c r="K33">
-        <v>-2.2343059613561E-3</v>
+        <v>-6.6195760861759406E-2</v>
       </c>
       <c r="L33">
-        <v>9.8216115109424594E-3</v>
+        <v>-4.9620274821055799E-2</v>
       </c>
       <c r="M33">
-        <v>-4.1358039133850702E-3</v>
+        <v>-6.7308511921754896E-2</v>
       </c>
       <c r="N33">
-        <v>2.6086044901671101E-3</v>
+        <v>-5.3466620786926398E-2</v>
       </c>
       <c r="O33">
-        <v>-4.2607702365087201E-2</v>
+        <v>-5.32256130875376E-2</v>
       </c>
       <c r="P33">
-        <v>-0.10080114369368801</v>
+        <v>-3.99429733484368E-2</v>
       </c>
       <c r="Q33">
-        <v>6.0654579068559103E-2</v>
+        <v>2.2024631149884601E-2</v>
       </c>
       <c r="R33">
-        <v>5.6099909861986499E-2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>1.88576238273837E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -4404,161 +4403,161 @@
         <v>0</v>
       </c>
       <c r="E34">
-        <v>0.40674837802394898</v>
+        <v>7.6483477973740402E-2</v>
       </c>
       <c r="F34">
-        <v>0.39264510260292101</v>
+        <v>6.6378371307455705E-2</v>
       </c>
       <c r="G34">
-        <v>0.34132538858477801</v>
+        <v>3.35910656759019E-2</v>
       </c>
       <c r="H34">
-        <v>0.324473156893754</v>
+        <v>1.08825872219125E-2</v>
       </c>
       <c r="I34">
-        <v>-0.101174962269748</v>
+        <v>-0.180946366559365</v>
       </c>
       <c r="J34">
-        <v>-8.9770109921996605E-2</v>
+        <v>-5.9771325791893898E-2</v>
       </c>
       <c r="K34">
-        <v>2.3336439450052E-2</v>
+        <v>-8.3394050863961497E-2</v>
       </c>
       <c r="L34">
-        <v>6.7646404324579095E-4</v>
+        <v>-6.8444094455491794E-2</v>
       </c>
       <c r="M34">
-        <v>0.122217159526473</v>
+        <v>-7.8950407659903604E-2</v>
       </c>
       <c r="N34">
-        <v>5.7214744458342702E-2</v>
+        <v>-7.2200572757733505E-2</v>
       </c>
       <c r="O34">
-        <v>5.8811056025830102E-2</v>
+        <v>-5.6154300841595797E-2</v>
       </c>
       <c r="P34">
-        <v>6.2870829543728801E-2</v>
+        <v>-5.5886103737597399E-2</v>
       </c>
       <c r="Q34">
-        <v>0.37763293389554098</v>
+        <v>2.2158949126526599E-2</v>
       </c>
       <c r="R34">
-        <v>0.22175060130858701</v>
-      </c>
-    </row>
-    <row r="35" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>1.8048159872860899E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>0.5</v>
       </c>
       <c r="B35">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="C35" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D35" t="s">
         <v>0</v>
       </c>
       <c r="E35">
-        <v>7.6483477973740402E-2</v>
+        <v>0.13669432419510499</v>
       </c>
       <c r="F35">
-        <v>6.6378371307455705E-2</v>
+        <v>0.133556422960978</v>
       </c>
       <c r="G35">
-        <v>3.35910656759019E-2</v>
+        <v>8.8034132684122093E-2</v>
       </c>
       <c r="H35">
-        <v>1.08825872219125E-2</v>
+        <v>4.76508951287926E-2</v>
       </c>
       <c r="I35">
-        <v>-0.180946366559365</v>
+        <v>-0.153740183381916</v>
       </c>
       <c r="J35">
-        <v>-5.9771325791893898E-2</v>
+        <v>-1.74943103340085E-2</v>
       </c>
       <c r="K35">
-        <v>-8.3394050863961497E-2</v>
+        <v>7.3984191122947504E-2</v>
       </c>
       <c r="L35">
-        <v>-6.8444094455491794E-2</v>
+        <v>8.2185218147474801E-2</v>
       </c>
       <c r="M35">
-        <v>-7.8950407659903604E-2</v>
+        <v>7.1212371225103793E-2</v>
       </c>
       <c r="N35">
-        <v>-7.2200572757733505E-2</v>
+        <v>7.6545987057850803E-2</v>
       </c>
       <c r="O35">
-        <v>-5.6154300841595797E-2</v>
+        <v>3.4300796276771697E-2</v>
       </c>
       <c r="P35">
-        <v>-5.5886103737597399E-2</v>
+        <v>1.5125065550481801E-2</v>
       </c>
       <c r="Q35">
-        <v>2.2158949126526599E-2</v>
+        <v>8.0583988135130805E-2</v>
       </c>
       <c r="R35">
-        <v>1.8048159872860899E-2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>7.7359228864058105E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="B36">
         <v>0.2</v>
       </c>
       <c r="C36" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D36" t="s">
         <v>0</v>
       </c>
       <c r="E36">
-        <v>0.42524918622058799</v>
+        <v>0.12181965733904</v>
       </c>
       <c r="F36">
-        <v>0.42003666060161199</v>
+        <v>0.115875322460899</v>
       </c>
       <c r="G36">
-        <v>0.35425757480871101</v>
+        <v>7.3244517179751306E-2</v>
       </c>
       <c r="H36">
-        <v>0.33314751577169399</v>
+        <v>3.0831589694546701E-2</v>
       </c>
       <c r="I36">
-        <v>-3.9451326042871201E-2</v>
+        <v>-0.16859766473228599</v>
       </c>
       <c r="J36">
-        <v>-2.4805310862793001E-2</v>
+        <v>-4.1722740165033301E-2</v>
       </c>
       <c r="K36">
-        <v>8.8992982801883294E-2</v>
+        <v>-2.2343059613561E-3</v>
       </c>
       <c r="L36">
-        <v>5.0310883541125402E-2</v>
+        <v>9.8216115109424594E-3</v>
       </c>
       <c r="M36">
-        <v>0.173348026120906</v>
+        <v>-4.1358039133850702E-3</v>
       </c>
       <c r="N36">
-        <v>8.6832566524164795E-2</v>
+        <v>2.6086044901671101E-3</v>
       </c>
       <c r="O36">
-        <v>2.22095365532517E-2</v>
+        <v>-4.2607702365087201E-2</v>
       </c>
       <c r="P36">
-        <v>3.8506265655108597E-2</v>
+        <v>-0.10080114369368801</v>
       </c>
       <c r="Q36">
-        <v>0.36375473227316302</v>
+        <v>6.0654579068559103E-2</v>
       </c>
       <c r="R36">
-        <v>0.241231551750235</v>
-      </c>
-    </row>
-    <row r="37" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>5.6099909861986499E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>0.5</v>
       </c>
@@ -4616,13 +4615,8 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:R37">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="med"/>
-      </filters>
-    </filterColumn>
-    <sortState ref="A14:R25">
-      <sortCondition ref="B1:B37"/>
+    <sortState ref="A26:R37">
+      <sortCondition ref="A1:A37"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4635,8 +4629,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="O20" sqref="O20:P22"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="Q32" sqref="Q32:Q37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5369,7 +5363,7 @@
         <v>7.3296462896105294E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0</v>
       </c>
@@ -5425,7 +5419,7 @@
         <v>0.14012604861399899</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0</v>
       </c>
@@ -5481,7 +5475,7 @@
         <v>0.21211201779057401</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>0</v>
       </c>
@@ -5537,7 +5531,7 @@
         <v>0.24183533854966399</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>0.5</v>
       </c>
@@ -5593,7 +5587,7 @@
         <v>3.4058241512594997E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>0.5</v>
       </c>
@@ -5649,7 +5643,7 @@
         <v>3.4393211327645098E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>0.5</v>
       </c>
@@ -5705,7 +5699,7 @@
         <v>3.45642696780908E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>0</v>
       </c>
@@ -5761,7 +5755,7 @@
         <v>0.215058359551489</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>0</v>
       </c>
@@ -5817,7 +5811,7 @@
         <v>0.24589633658593099</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>0</v>
       </c>
@@ -5873,7 +5867,7 @@
         <v>0.24992502306624401</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>0.5</v>
       </c>
@@ -5929,7 +5923,7 @@
         <v>7.9403975227007595E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>0.5</v>
       </c>
@@ -5985,7 +5979,7 @@
         <v>6.4486932443238804E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>0.5</v>
       </c>
@@ -6041,7 +6035,7 @@
         <v>6.35376312768135E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>0</v>
       </c>
@@ -6097,121 +6091,121 @@
         <v>0.25885525890701599</v>
       </c>
     </row>
-    <row r="27" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="B27">
         <v>0</v>
       </c>
       <c r="C27" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D27" t="s">
         <v>0</v>
       </c>
       <c r="E27">
-        <v>9.0616784872585898E-2</v>
+        <v>0.385848503370949</v>
       </c>
       <c r="F27">
-        <v>6.6136803692062707E-2</v>
+        <v>0.36963979900791</v>
       </c>
       <c r="G27">
-        <v>7.2272294239484294E-2</v>
+        <v>0.32233900495783102</v>
       </c>
       <c r="H27">
-        <v>2.64505682125919E-2</v>
+        <v>0.30467342859665902</v>
       </c>
       <c r="I27">
-        <v>0.26831263196772898</v>
+        <v>0.19997580522094699</v>
       </c>
       <c r="J27">
-        <v>6.4549262299600493E-2</v>
+        <v>0.104741695609101</v>
       </c>
       <c r="K27">
-        <v>9.1882915311988195E-2</v>
+        <v>7.1788883937242504E-2</v>
       </c>
       <c r="L27">
-        <v>3.4211028450356999E-2</v>
+        <v>8.7922338744301099E-3</v>
       </c>
       <c r="M27">
-        <v>8.8974582706680197E-2</v>
+        <v>0.146794039205974</v>
       </c>
       <c r="N27">
-        <v>3.3402111265170703E-2</v>
+        <v>5.3334065628869998E-2</v>
       </c>
       <c r="O27">
-        <v>8.5170839594355105E-2</v>
+        <v>9.0266885474818204E-2</v>
       </c>
       <c r="P27">
-        <v>3.10439755710313E-2</v>
+        <v>5.3887578019350103E-2</v>
       </c>
       <c r="Q27">
-        <v>7.4422064432359603E-2</v>
+        <v>0.36042487183168598</v>
       </c>
       <c r="R27">
-        <v>3.4837127925387901E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>0.23337255525068601</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>0</v>
       </c>
       <c r="B28">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C28" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D28" t="s">
         <v>0</v>
       </c>
       <c r="E28">
-        <v>0.39377269896893202</v>
+        <v>0.41190720493080202</v>
       </c>
       <c r="F28">
-        <v>0.390815416329021</v>
+        <v>0.39346321578492599</v>
       </c>
       <c r="G28">
-        <v>0.33636605938094299</v>
+        <v>0.34821607423628298</v>
       </c>
       <c r="H28">
-        <v>0.30411260046240501</v>
+        <v>0.32551948195012997</v>
       </c>
       <c r="I28">
-        <v>0.32929677705501798</v>
+        <v>0.19407402716494501</v>
       </c>
       <c r="J28">
-        <v>0.19237086458351901</v>
+        <v>0.10432959365743601</v>
       </c>
       <c r="K28">
-        <v>0.29277584823348302</v>
+        <v>6.5519550367572899E-2</v>
       </c>
       <c r="L28">
-        <v>0.275332874449081</v>
+        <v>6.27140415791073E-3</v>
       </c>
       <c r="M28">
-        <v>0.30395183300453599</v>
+        <v>0.148018477441272</v>
       </c>
       <c r="N28">
-        <v>0.27413087541035602</v>
+        <v>6.6194509442864202E-2</v>
       </c>
       <c r="O28">
-        <v>0.25783380962883601</v>
+        <v>7.6920597772740101E-2</v>
       </c>
       <c r="P28">
-        <v>0.16620316601856899</v>
+        <v>6.6669221474724705E-2</v>
       </c>
       <c r="Q28">
-        <v>0.34836252987842198</v>
+        <v>0.38503035837042299</v>
       </c>
       <c r="R28">
-        <v>0.27266711470595401</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>0.230311278199441</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="B29">
         <v>0.2</v>
@@ -6223,54 +6217,54 @@
         <v>0</v>
       </c>
       <c r="E29">
-        <v>0.157481054544684</v>
+        <v>0.39377269896893202</v>
       </c>
       <c r="F29">
-        <v>0.13700862343984699</v>
+        <v>0.390815416329021</v>
       </c>
       <c r="G29">
-        <v>0.13063506205247699</v>
+        <v>0.33636605938094299</v>
       </c>
       <c r="H29">
-        <v>6.45136721367634E-2</v>
+        <v>0.30411260046240501</v>
       </c>
       <c r="I29">
-        <v>0.31255420864934802</v>
+        <v>0.32929677705501798</v>
       </c>
       <c r="J29">
-        <v>8.4688625504924203E-2</v>
+        <v>0.19237086458351901</v>
       </c>
       <c r="K29">
-        <v>0.138450089983221</v>
+        <v>0.29277584823348302</v>
       </c>
       <c r="L29">
-        <v>9.26091147766578E-2</v>
+        <v>0.275332874449081</v>
       </c>
       <c r="M29">
-        <v>0.13202653821584101</v>
+        <v>0.30395183300453599</v>
       </c>
       <c r="N29">
-        <v>8.7390518833409397E-2</v>
+        <v>0.27413087541035602</v>
       </c>
       <c r="O29">
-        <v>0.12603074278388801</v>
+        <v>0.25783380962883601</v>
       </c>
       <c r="P29">
-        <v>6.4601819097522703E-2</v>
+        <v>0.16620316601856899</v>
       </c>
       <c r="Q29">
-        <v>0.13124654569704799</v>
+        <v>0.34836252987842198</v>
       </c>
       <c r="R29">
-        <v>8.9336795163627594E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>0.27266711470595401</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>0</v>
       </c>
       <c r="B30">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="C30" t="s">
         <v>1</v>
@@ -6279,166 +6273,166 @@
         <v>0</v>
       </c>
       <c r="E30">
-        <v>0.385848503370949</v>
+        <v>0.41914501185583403</v>
       </c>
       <c r="F30">
-        <v>0.36963979900791</v>
+        <v>0.41170229658539398</v>
       </c>
       <c r="G30">
-        <v>0.32233900495783102</v>
+        <v>0.35340938652186599</v>
       </c>
       <c r="H30">
-        <v>0.30467342859665902</v>
+        <v>0.32669538175359603</v>
       </c>
       <c r="I30">
-        <v>0.19997580522094699</v>
+        <v>0.30311672827157399</v>
       </c>
       <c r="J30">
-        <v>0.104741695609101</v>
+        <v>0.145845777552532</v>
       </c>
       <c r="K30">
-        <v>7.1788883937242504E-2</v>
+        <v>0.17524101028495701</v>
       </c>
       <c r="L30">
-        <v>8.7922338744301099E-3</v>
+        <v>0.11689319782948</v>
       </c>
       <c r="M30">
-        <v>0.146794039205974</v>
+        <v>0.21435240212977599</v>
       </c>
       <c r="N30">
-        <v>5.3334065628869998E-2</v>
+        <v>0.12951251257740901</v>
       </c>
       <c r="O30">
-        <v>9.0266885474818204E-2</v>
+        <v>0.19335123603558901</v>
       </c>
       <c r="P30">
-        <v>5.3887578019350103E-2</v>
+        <v>9.5822625300144001E-2</v>
       </c>
       <c r="Q30">
-        <v>0.36042487183168598</v>
+        <v>0.36876473892853801</v>
       </c>
       <c r="R30">
-        <v>0.23337255525068601</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>0.26889627652882397</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31">
+        <v>0</v>
+      </c>
+      <c r="B31">
+        <v>0.2</v>
+      </c>
+      <c r="C31" t="s">
+        <v>0</v>
+      </c>
+      <c r="D31" t="s">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0.43066770604122301</v>
+      </c>
+      <c r="F31">
+        <v>0.42077881025346198</v>
+      </c>
+      <c r="G31">
+        <v>0.36447415077927298</v>
+      </c>
+      <c r="H31">
+        <v>0.33448887748055101</v>
+      </c>
+      <c r="I31">
+        <v>0.28582137363303201</v>
+      </c>
+      <c r="J31">
+        <v>0.14727107944295201</v>
+      </c>
+      <c r="K31">
+        <v>0.14523713410195199</v>
+      </c>
+      <c r="L31">
+        <v>7.8039417139741094E-2</v>
+      </c>
+      <c r="M31">
+        <v>0.20024381579841999</v>
+      </c>
+      <c r="N31">
+        <v>0.101229613838761</v>
+      </c>
+      <c r="O31">
+        <v>0.16406082865410901</v>
+      </c>
+      <c r="P31">
+        <v>9.1364044840528694E-2</v>
+      </c>
+      <c r="Q31">
+        <v>0.37547278961954</v>
+      </c>
+      <c r="R31">
+        <v>0.265964824990436</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A32">
         <v>0.5</v>
       </c>
-      <c r="B31">
-        <v>0</v>
-      </c>
-      <c r="C31" t="s">
-        <v>1</v>
-      </c>
-      <c r="D31" t="s">
-        <v>0</v>
-      </c>
-      <c r="E31">
-        <v>9.2758696964963305E-2</v>
-      </c>
-      <c r="F31">
-        <v>6.92701963238362E-2</v>
-      </c>
-      <c r="G31">
-        <v>7.3627214245878703E-2</v>
-      </c>
-      <c r="H31">
-        <v>2.7991807083577399E-2</v>
-      </c>
-      <c r="I31">
-        <v>0.27342361870388399</v>
-      </c>
-      <c r="J31">
-        <v>6.8711909330540194E-2</v>
-      </c>
-      <c r="K31">
-        <v>0.13750273643174599</v>
-      </c>
-      <c r="L31">
-        <v>6.5642790438606394E-2</v>
-      </c>
-      <c r="M31">
-        <v>0.130337985716827</v>
-      </c>
-      <c r="N31">
-        <v>6.7780265487904501E-2</v>
-      </c>
-      <c r="O31">
-        <v>9.7103920425974599E-2</v>
-      </c>
-      <c r="P31">
-        <v>5.6434748796041802E-2</v>
-      </c>
-      <c r="Q31">
-        <v>7.5070820513781902E-2</v>
-      </c>
-      <c r="R31">
-        <v>3.5168440920095703E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>0</v>
-      </c>
       <c r="B32">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C32" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D32" t="s">
         <v>0</v>
       </c>
       <c r="E32">
-        <v>0.41914501185583403</v>
+        <v>9.0616784872585898E-2</v>
       </c>
       <c r="F32">
-        <v>0.41170229658539398</v>
+        <v>6.6136803692062707E-2</v>
       </c>
       <c r="G32">
-        <v>0.35340938652186599</v>
+        <v>7.2272294239484294E-2</v>
       </c>
       <c r="H32">
-        <v>0.32669538175359603</v>
+        <v>2.64505682125919E-2</v>
       </c>
       <c r="I32">
-        <v>0.30311672827157399</v>
+        <v>0.26831263196772898</v>
       </c>
       <c r="J32">
-        <v>0.145845777552532</v>
+        <v>6.4549262299600493E-2</v>
       </c>
       <c r="K32">
-        <v>0.17524101028495701</v>
+        <v>9.1882915311988195E-2</v>
       </c>
       <c r="L32">
-        <v>0.11689319782948</v>
+        <v>3.4211028450356999E-2</v>
       </c>
       <c r="M32">
-        <v>0.21435240212977599</v>
+        <v>8.8974582706680197E-2</v>
       </c>
       <c r="N32">
-        <v>0.12951251257740901</v>
+        <v>3.3402111265170703E-2</v>
       </c>
       <c r="O32">
-        <v>0.19335123603558901</v>
+        <v>8.5170839594355105E-2</v>
       </c>
       <c r="P32">
-        <v>9.5822625300144001E-2</v>
+        <v>3.10439755710313E-2</v>
       </c>
       <c r="Q32">
-        <v>0.36876473892853801</v>
+        <v>7.4422064432359603E-2</v>
       </c>
       <c r="R32">
-        <v>0.26889627652882397</v>
-      </c>
-    </row>
-    <row r="33" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>3.4837127925387901E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>0.5</v>
       </c>
       <c r="B33">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C33" t="s">
         <v>1</v>
@@ -6447,51 +6441,51 @@
         <v>0</v>
       </c>
       <c r="E33">
-        <v>0.14453967822036701</v>
+        <v>9.2758696964963305E-2</v>
       </c>
       <c r="F33">
-        <v>0.119985279134943</v>
+        <v>6.92701963238362E-2</v>
       </c>
       <c r="G33">
-        <v>0.12012541457548601</v>
+        <v>7.3627214245878703E-2</v>
       </c>
       <c r="H33">
-        <v>5.2672814512440297E-2</v>
+        <v>2.7991807083577399E-2</v>
       </c>
       <c r="I33">
-        <v>0.31428887170208197</v>
+        <v>0.27342361870388399</v>
       </c>
       <c r="J33">
-        <v>0.102262963540364</v>
+        <v>6.8711909330540194E-2</v>
       </c>
       <c r="K33">
-        <v>0.14029352860441399</v>
+        <v>0.13750273643174599</v>
       </c>
       <c r="L33">
-        <v>5.1320094874137898E-2</v>
+        <v>6.5642790438606394E-2</v>
       </c>
       <c r="M33">
-        <v>0.13108453194872699</v>
+        <v>0.130337985716827</v>
       </c>
       <c r="N33">
-        <v>5.0913286685377299E-2</v>
+        <v>6.7780265487904501E-2</v>
       </c>
       <c r="O33">
-        <v>0.15021876367620399</v>
+        <v>9.7103920425974599E-2</v>
       </c>
       <c r="P33">
-        <v>0.138417594459737</v>
+        <v>5.6434748796041802E-2</v>
       </c>
       <c r="Q33">
-        <v>0.12168938198281901</v>
+        <v>7.5070820513781902E-2</v>
       </c>
       <c r="R33">
-        <v>7.2641514392633305E-2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>3.5168440920095703E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -6503,161 +6497,161 @@
         <v>0</v>
       </c>
       <c r="E34">
-        <v>0.41190720493080202</v>
+        <v>9.4652708195794702E-2</v>
       </c>
       <c r="F34">
-        <v>0.39346321578492599</v>
+        <v>7.0129096160672505E-2</v>
       </c>
       <c r="G34">
-        <v>0.34821607423628298</v>
+        <v>7.2977483094140302E-2</v>
       </c>
       <c r="H34">
-        <v>0.32551948195012997</v>
+        <v>2.80752991538957E-2</v>
       </c>
       <c r="I34">
-        <v>0.19407402716494501</v>
+        <v>0.28447471507701899</v>
       </c>
       <c r="J34">
-        <v>0.10432959365743601</v>
+        <v>7.1844439488032402E-2</v>
       </c>
       <c r="K34">
-        <v>6.5519550367572899E-2</v>
+        <v>0.15836299311260901</v>
       </c>
       <c r="L34">
-        <v>6.27140415791073E-3</v>
+        <v>8.2843841717359298E-2</v>
       </c>
       <c r="M34">
-        <v>0.148018477441272</v>
+        <v>0.143382299233483</v>
       </c>
       <c r="N34">
-        <v>6.6194509442864202E-2</v>
+        <v>8.5585163918059606E-2</v>
       </c>
       <c r="O34">
-        <v>7.6920597772740101E-2</v>
+        <v>0.11268527746373901</v>
       </c>
       <c r="P34">
-        <v>6.6669221474724705E-2</v>
+        <v>7.6369348584826302E-2</v>
       </c>
       <c r="Q34">
-        <v>0.38503035837042299</v>
+        <v>7.4467935614955003E-2</v>
       </c>
       <c r="R34">
-        <v>0.230311278199441</v>
-      </c>
-    </row>
-    <row r="35" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>3.42866921461593E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>0.5</v>
       </c>
       <c r="B35">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="C35" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D35" t="s">
         <v>0</v>
       </c>
       <c r="E35">
-        <v>9.4652708195794702E-2</v>
+        <v>0.157481054544684</v>
       </c>
       <c r="F35">
-        <v>7.0129096160672505E-2</v>
+        <v>0.13700862343984699</v>
       </c>
       <c r="G35">
-        <v>7.2977483094140302E-2</v>
+        <v>0.13063506205247699</v>
       </c>
       <c r="H35">
-        <v>2.80752991538957E-2</v>
+        <v>6.45136721367634E-2</v>
       </c>
       <c r="I35">
-        <v>0.28447471507701899</v>
+        <v>0.31255420864934802</v>
       </c>
       <c r="J35">
-        <v>7.1844439488032402E-2</v>
+        <v>8.4688625504924203E-2</v>
       </c>
       <c r="K35">
-        <v>0.15836299311260901</v>
+        <v>0.138450089983221</v>
       </c>
       <c r="L35">
-        <v>8.2843841717359298E-2</v>
+        <v>9.26091147766578E-2</v>
       </c>
       <c r="M35">
-        <v>0.143382299233483</v>
+        <v>0.13202653821584101</v>
       </c>
       <c r="N35">
-        <v>8.5585163918059606E-2</v>
+        <v>8.7390518833409397E-2</v>
       </c>
       <c r="O35">
-        <v>0.11268527746373901</v>
+        <v>0.12603074278388801</v>
       </c>
       <c r="P35">
-        <v>7.6369348584826302E-2</v>
+        <v>6.4601819097522703E-2</v>
       </c>
       <c r="Q35">
-        <v>7.4467935614955003E-2</v>
+        <v>0.13124654569704799</v>
       </c>
       <c r="R35">
-        <v>3.42866921461593E-2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>8.9336795163627594E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="B36">
         <v>0.2</v>
       </c>
       <c r="C36" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D36" t="s">
         <v>0</v>
       </c>
       <c r="E36">
-        <v>0.43066770604122301</v>
+        <v>0.14453967822036701</v>
       </c>
       <c r="F36">
-        <v>0.42077881025346198</v>
+        <v>0.119985279134943</v>
       </c>
       <c r="G36">
-        <v>0.36447415077927298</v>
+        <v>0.12012541457548601</v>
       </c>
       <c r="H36">
-        <v>0.33448887748055101</v>
+        <v>5.2672814512440297E-2</v>
       </c>
       <c r="I36">
-        <v>0.28582137363303201</v>
+        <v>0.31428887170208197</v>
       </c>
       <c r="J36">
-        <v>0.14727107944295201</v>
+        <v>0.102262963540364</v>
       </c>
       <c r="K36">
-        <v>0.14523713410195199</v>
+        <v>0.14029352860441399</v>
       </c>
       <c r="L36">
-        <v>7.8039417139741094E-2</v>
+        <v>5.1320094874137898E-2</v>
       </c>
       <c r="M36">
-        <v>0.20024381579841999</v>
+        <v>0.13108453194872699</v>
       </c>
       <c r="N36">
-        <v>0.101229613838761</v>
+        <v>5.0913286685377299E-2</v>
       </c>
       <c r="O36">
-        <v>0.16406082865410901</v>
+        <v>0.15021876367620399</v>
       </c>
       <c r="P36">
-        <v>9.1364044840528694E-2</v>
+        <v>0.138417594459737</v>
       </c>
       <c r="Q36">
-        <v>0.37547278961954</v>
+        <v>0.12168938198281901</v>
       </c>
       <c r="R36">
-        <v>0.265964824990436</v>
-      </c>
-    </row>
-    <row r="37" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>7.2641514392633305E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>0.5</v>
       </c>
@@ -6717,11 +6711,11 @@
   <autoFilter ref="A1:R37">
     <filterColumn colId="3">
       <filters>
-        <filter val="med"/>
+        <filter val="high"/>
       </filters>
     </filterColumn>
-    <sortState ref="A14:R25">
-      <sortCondition ref="B1:B37"/>
+    <sortState ref="A26:R37">
+      <sortCondition ref="A1:A37"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6733,8 +6727,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="O14" sqref="O14:P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7637,10 +7631,10 @@
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
@@ -7649,22 +7643,22 @@
         <v>1</v>
       </c>
       <c r="E17" s="2">
-        <v>0.89</v>
+        <v>0.375</v>
       </c>
       <c r="F17" s="2">
-        <v>0.43</v>
+        <v>0</v>
       </c>
       <c r="G17" s="2">
-        <v>0.91691995947315097</v>
+        <v>0.48542713567839202</v>
       </c>
       <c r="H17" s="2">
-        <v>0.88278008298755195</v>
+        <v>0.14699999999999999</v>
       </c>
       <c r="I17" s="2">
-        <v>0.875</v>
+        <v>0.84899999999999998</v>
       </c>
       <c r="J17" s="2">
-        <v>0.78500000000000003</v>
+        <v>0.73299999999999998</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>21</v>
@@ -7673,30 +7667,30 @@
         <v>21</v>
       </c>
       <c r="M17" s="2">
-        <v>0.94594594594594605</v>
+        <v>0.72574850299401195</v>
       </c>
       <c r="N17" s="2">
-        <v>0.95</v>
+        <v>0.237713139418255</v>
       </c>
       <c r="O17" s="2">
-        <v>0.92531120331950201</v>
+        <v>0.74472361809045196</v>
       </c>
       <c r="P17" s="2">
-        <v>0.94899999999999995</v>
+        <v>0.55400000000000005</v>
       </c>
       <c r="Q17" s="2">
-        <v>0.89800000000000002</v>
+        <v>0.47699999999999998</v>
       </c>
       <c r="R17" s="2">
-        <v>0.85799999999999998</v>
+        <v>0.111</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="C18" t="s">
         <v>1</v>
@@ -7705,22 +7699,22 @@
         <v>1</v>
       </c>
       <c r="E18" s="2">
-        <v>0.879</v>
+        <v>0.21199999999999999</v>
       </c>
       <c r="F18" s="2">
-        <v>0.26300000000000001</v>
+        <v>0</v>
       </c>
       <c r="G18" s="2">
-        <v>0.92016376663254895</v>
+        <v>0.40201005025125602</v>
       </c>
       <c r="H18" s="2">
-        <v>0.910064239828694</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="I18" s="2">
-        <v>0.79</v>
+        <v>0.871</v>
       </c>
       <c r="J18" s="2">
-        <v>0.57199999999999995</v>
+        <v>0.77100000000000002</v>
       </c>
       <c r="K18" s="2" t="s">
         <v>21</v>
@@ -7729,30 +7723,30 @@
         <v>21</v>
       </c>
       <c r="M18" s="2">
-        <v>0.917933130699088</v>
+        <v>0.91185897435897401</v>
       </c>
       <c r="N18" s="2">
-        <v>0.746</v>
+        <v>0.81176470588235305</v>
       </c>
       <c r="O18" s="2">
-        <v>0.93604651162790697</v>
+        <v>0.84879032258064502</v>
       </c>
       <c r="P18" s="2">
-        <v>0.93378226711559997</v>
+        <v>0.81399999999999995</v>
       </c>
       <c r="Q18" s="2">
-        <v>0.93500000000000005</v>
+        <v>0.41499999999999998</v>
       </c>
       <c r="R18" s="2">
-        <v>0.86699999999999999</v>
+        <v>0.19600000000000001</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="C19" t="s">
         <v>0</v>
@@ -7761,22 +7755,22 @@
         <v>1</v>
       </c>
       <c r="E19" s="2">
-        <v>0.86599999999999999</v>
+        <v>0.156</v>
       </c>
       <c r="F19" s="2">
-        <v>0.24199999999999999</v>
+        <v>0</v>
       </c>
       <c r="G19" s="2">
-        <v>0.92805755395683498</v>
+        <v>0.33366935483871002</v>
       </c>
       <c r="H19" s="2">
-        <v>0.918432203389831</v>
+        <v>0</v>
       </c>
       <c r="I19" s="2">
-        <v>0.74299999999999999</v>
+        <v>0.85</v>
       </c>
       <c r="J19" s="2">
-        <v>0.505</v>
+        <v>0.64500000000000002</v>
       </c>
       <c r="K19" s="2" t="s">
         <v>21</v>
@@ -7785,30 +7779,30 @@
         <v>21</v>
       </c>
       <c r="M19" s="2">
-        <v>0.920282542885974</v>
+        <v>0.92351816443594603</v>
       </c>
       <c r="N19" s="2">
-        <v>0.61799999999999999</v>
+        <v>0.90328151986183103</v>
       </c>
       <c r="O19" s="2">
-        <v>0.91925465838509302</v>
+        <v>0.82914046121593299</v>
       </c>
       <c r="P19" s="2">
-        <v>0.91472868217054304</v>
+        <v>0.79400000000000004</v>
       </c>
       <c r="Q19" s="2">
-        <v>0.91900000000000004</v>
+        <v>0.377</v>
       </c>
       <c r="R19" s="2">
-        <v>0.86199999999999999</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="B20">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C20" t="s">
         <v>2</v>
@@ -7817,22 +7811,22 @@
         <v>1</v>
       </c>
       <c r="E20" s="2">
-        <v>0.375</v>
+        <v>0.89</v>
       </c>
       <c r="F20" s="2">
-        <v>0</v>
+        <v>0.43</v>
       </c>
       <c r="G20" s="2">
-        <v>0.48542713567839202</v>
+        <v>0.91691995947315097</v>
       </c>
       <c r="H20" s="2">
-        <v>0.14699999999999999</v>
+        <v>0.88278008298755195</v>
       </c>
       <c r="I20" s="2">
-        <v>0.84899999999999998</v>
+        <v>0.875</v>
       </c>
       <c r="J20" s="2">
-        <v>0.73299999999999998</v>
+        <v>0.78500000000000003</v>
       </c>
       <c r="K20" s="2" t="s">
         <v>21</v>
@@ -7841,30 +7835,30 @@
         <v>21</v>
       </c>
       <c r="M20" s="2">
-        <v>0.72574850299401195</v>
+        <v>0.94594594594594605</v>
       </c>
       <c r="N20" s="2">
-        <v>0.237713139418255</v>
+        <v>0.95</v>
       </c>
       <c r="O20" s="2">
-        <v>0.74472361809045196</v>
+        <v>0.92531120331950201</v>
       </c>
       <c r="P20" s="2">
-        <v>0.55400000000000005</v>
+        <v>0.94899999999999995</v>
       </c>
       <c r="Q20" s="2">
-        <v>0.47699999999999998</v>
+        <v>0.89800000000000002</v>
       </c>
       <c r="R20" s="2">
-        <v>0.111</v>
+        <v>0.85799999999999998</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="B21">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C21" t="s">
         <v>1</v>
@@ -7873,22 +7867,22 @@
         <v>1</v>
       </c>
       <c r="E21" s="2">
-        <v>0.21199999999999999</v>
+        <v>0.879</v>
       </c>
       <c r="F21" s="2">
-        <v>0</v>
+        <v>0.26300000000000001</v>
       </c>
       <c r="G21" s="2">
-        <v>0.40201005025125602</v>
+        <v>0.92016376663254895</v>
       </c>
       <c r="H21" s="2">
-        <v>7.0000000000000001E-3</v>
+        <v>0.910064239828694</v>
       </c>
       <c r="I21" s="2">
-        <v>0.871</v>
+        <v>0.79</v>
       </c>
       <c r="J21" s="2">
-        <v>0.77100000000000002</v>
+        <v>0.57199999999999995</v>
       </c>
       <c r="K21" s="2" t="s">
         <v>21</v>
@@ -7897,30 +7891,30 @@
         <v>21</v>
       </c>
       <c r="M21" s="2">
-        <v>0.91185897435897401</v>
+        <v>0.917933130699088</v>
       </c>
       <c r="N21" s="2">
-        <v>0.81176470588235305</v>
+        <v>0.746</v>
       </c>
       <c r="O21" s="2">
-        <v>0.84879032258064502</v>
+        <v>0.93604651162790697</v>
       </c>
       <c r="P21" s="2">
-        <v>0.81399999999999995</v>
+        <v>0.93378226711559997</v>
       </c>
       <c r="Q21" s="2">
-        <v>0.41499999999999998</v>
+        <v>0.93500000000000005</v>
       </c>
       <c r="R21" s="2">
-        <v>0.19600000000000001</v>
+        <v>0.86699999999999999</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="B22">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C22" t="s">
         <v>0</v>
@@ -7929,22 +7923,22 @@
         <v>1</v>
       </c>
       <c r="E22" s="2">
-        <v>0.156</v>
+        <v>0.86599999999999999</v>
       </c>
       <c r="F22" s="2">
-        <v>0</v>
+        <v>0.24199999999999999</v>
       </c>
       <c r="G22" s="2">
-        <v>0.33366935483871002</v>
+        <v>0.92805755395683498</v>
       </c>
       <c r="H22" s="2">
-        <v>0</v>
+        <v>0.918432203389831</v>
       </c>
       <c r="I22" s="2">
-        <v>0.85</v>
+        <v>0.74299999999999999</v>
       </c>
       <c r="J22" s="2">
-        <v>0.64500000000000002</v>
+        <v>0.505</v>
       </c>
       <c r="K22" s="2" t="s">
         <v>21</v>
@@ -7953,22 +7947,22 @@
         <v>21</v>
       </c>
       <c r="M22" s="2">
-        <v>0.92351816443594603</v>
+        <v>0.920282542885974</v>
       </c>
       <c r="N22" s="2">
-        <v>0.90328151986183103</v>
+        <v>0.61799999999999999</v>
       </c>
       <c r="O22" s="2">
-        <v>0.82914046121593299</v>
+        <v>0.91925465838509302</v>
       </c>
       <c r="P22" s="2">
-        <v>0.79400000000000004</v>
+        <v>0.91472868217054304</v>
       </c>
       <c r="Q22" s="2">
-        <v>0.377</v>
+        <v>0.91900000000000004</v>
       </c>
       <c r="R22" s="2">
-        <v>0.22</v>
+        <v>0.86199999999999999</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
@@ -8197,34 +8191,34 @@
     </row>
     <row r="27" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="B27">
         <v>0</v>
       </c>
       <c r="C27" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D27" t="s">
         <v>0</v>
       </c>
       <c r="E27">
-        <v>0.82099999999999995</v>
+        <v>0</v>
       </c>
       <c r="F27">
-        <v>0.23</v>
+        <v>0</v>
       </c>
       <c r="G27">
-        <v>0.91277890466531397</v>
+        <v>2.8513238289205701E-2</v>
       </c>
       <c r="H27">
-        <v>0.91062039957939001</v>
+        <v>0</v>
       </c>
       <c r="I27">
-        <v>0.80500000000000005</v>
+        <v>0.88100000000000001</v>
       </c>
       <c r="J27">
-        <v>0.622</v>
+        <v>0.67400000000000004</v>
       </c>
       <c r="K27" t="s">
         <v>21</v>
@@ -8233,22 +8227,22 @@
         <v>21</v>
       </c>
       <c r="M27">
-        <v>0.96</v>
+        <v>0.99095022624434403</v>
       </c>
       <c r="N27">
-        <v>0.94899999999999995</v>
+        <v>1</v>
       </c>
       <c r="O27">
-        <v>0.94488188976377996</v>
+        <v>0.93742889647326499</v>
       </c>
       <c r="P27">
-        <v>0.960498960498961</v>
+        <v>0.88500000000000001</v>
       </c>
       <c r="Q27">
-        <v>0.89200000000000002</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="R27">
-        <v>0.81899999999999995</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="28" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
@@ -8256,31 +8250,31 @@
         <v>0</v>
       </c>
       <c r="B28">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C28" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D28" t="s">
         <v>0</v>
       </c>
       <c r="E28">
-        <v>5.3999999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="F28">
         <v>0</v>
       </c>
       <c r="G28">
-        <v>0.18960244648318</v>
+        <v>1.14107883817427E-2</v>
       </c>
       <c r="H28">
         <v>0</v>
       </c>
       <c r="I28">
-        <v>0.79600000000000004</v>
+        <v>0.873</v>
       </c>
       <c r="J28">
-        <v>0.63200000000000001</v>
+        <v>0.54800000000000004</v>
       </c>
       <c r="K28" t="s">
         <v>21</v>
@@ -8289,27 +8283,27 @@
         <v>21</v>
       </c>
       <c r="M28">
-        <v>0.62869660460021903</v>
+        <v>0.98404255319148903</v>
       </c>
       <c r="N28">
-        <v>5.9059059059059102E-2</v>
+        <v>1</v>
       </c>
       <c r="O28">
-        <v>0.54814814814814805</v>
+        <v>0.96619718309859204</v>
       </c>
       <c r="P28">
-        <v>0.47299999999999998</v>
+        <v>0.88688688688688699</v>
       </c>
       <c r="Q28">
-        <v>0.35899999999999999</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="R28">
-        <v>0.26100000000000001</v>
+        <v>0.26600000000000001</v>
       </c>
     </row>
     <row r="29" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="B29">
         <v>0.2</v>
@@ -8321,22 +8315,22 @@
         <v>0</v>
       </c>
       <c r="E29">
-        <v>0.54300000000000004</v>
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="F29">
-        <v>4.0000000000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="G29">
-        <v>0.69520897043832797</v>
+        <v>0.18960244648318</v>
       </c>
       <c r="H29">
-        <v>0.66581956797967001</v>
+        <v>0</v>
       </c>
       <c r="I29">
         <v>0.79600000000000004</v>
       </c>
       <c r="J29">
-        <v>0.82499999999999996</v>
+        <v>0.63200000000000001</v>
       </c>
       <c r="K29" t="s">
         <v>21</v>
@@ -8345,22 +8339,22 @@
         <v>21</v>
       </c>
       <c r="M29">
-        <v>0.83867735470941895</v>
+        <v>0.62869660460021903</v>
       </c>
       <c r="N29">
-        <v>0.497</v>
+        <v>5.9059059059059102E-2</v>
       </c>
       <c r="O29">
-        <v>0.83689839572192504</v>
+        <v>0.54814814814814805</v>
       </c>
       <c r="P29">
-        <v>0.89716684155299098</v>
+        <v>0.47299999999999998</v>
       </c>
       <c r="Q29">
-        <v>0.79</v>
+        <v>0.35899999999999999</v>
       </c>
       <c r="R29">
-        <v>0.40799999999999997</v>
+        <v>0.26100000000000001</v>
       </c>
     </row>
     <row r="30" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
@@ -8368,7 +8362,7 @@
         <v>0</v>
       </c>
       <c r="B30">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="C30" t="s">
         <v>1</v>
@@ -8377,22 +8371,22 @@
         <v>0</v>
       </c>
       <c r="E30">
-        <v>0</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="F30">
         <v>0</v>
       </c>
       <c r="G30">
-        <v>2.8513238289205701E-2</v>
+        <v>0.116182572614108</v>
       </c>
       <c r="H30">
         <v>0</v>
       </c>
       <c r="I30">
-        <v>0.88100000000000001</v>
+        <v>0.83099999999999996</v>
       </c>
       <c r="J30">
-        <v>0.67400000000000004</v>
+        <v>0.76900000000000002</v>
       </c>
       <c r="K30" t="s">
         <v>21</v>
@@ -8401,54 +8395,54 @@
         <v>21</v>
       </c>
       <c r="M30">
-        <v>0.99095022624434403</v>
+        <v>0.89076923076923098</v>
       </c>
       <c r="N30">
-        <v>1</v>
+        <v>0.75438596491228105</v>
       </c>
       <c r="O30">
-        <v>0.93742889647326499</v>
+        <v>0.78286558345642498</v>
       </c>
       <c r="P30">
-        <v>0.88500000000000001</v>
+        <v>0.84884884884884904</v>
       </c>
       <c r="Q30">
-        <v>5.7000000000000002E-2</v>
+        <v>0.29099999999999998</v>
       </c>
       <c r="R30">
-        <v>0.37</v>
+        <v>0.28000000000000003</v>
       </c>
     </row>
     <row r="31" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="B31">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="C31" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D31" t="s">
         <v>0</v>
       </c>
       <c r="E31">
-        <v>0.86199999999999999</v>
+        <v>0.01</v>
       </c>
       <c r="F31">
-        <v>0.221</v>
+        <v>0</v>
       </c>
       <c r="G31">
-        <v>0.92008196721311497</v>
+        <v>7.6053442959917797E-2</v>
       </c>
       <c r="H31">
-        <v>0.89669861554845598</v>
+        <v>0</v>
       </c>
       <c r="I31">
-        <v>0.752</v>
+        <v>0.84099999999999997</v>
       </c>
       <c r="J31">
-        <v>0.51600000000000001</v>
+        <v>0.76600000000000001</v>
       </c>
       <c r="K31" t="s">
         <v>21</v>
@@ -8457,54 +8451,54 @@
         <v>21</v>
       </c>
       <c r="M31">
-        <v>0.91356783919597995</v>
+        <v>0.92084942084942101</v>
       </c>
       <c r="N31">
-        <v>0.72199999999999998</v>
+        <v>0.90756302521008403</v>
       </c>
       <c r="O31">
-        <v>0.93693693693693703</v>
+        <v>0.82196969696969702</v>
       </c>
       <c r="P31">
-        <v>0.94017094017094005</v>
+        <v>0.76161616161616197</v>
       </c>
       <c r="Q31">
-        <v>0.92700000000000005</v>
+        <v>0.29899999999999999</v>
       </c>
       <c r="R31">
-        <v>0.84199999999999997</v>
+        <v>0.28599999999999998</v>
       </c>
     </row>
     <row r="32" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="B32">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C32" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D32" t="s">
         <v>0</v>
       </c>
       <c r="E32">
-        <v>1.4999999999999999E-2</v>
+        <v>0.82099999999999995</v>
       </c>
       <c r="F32">
-        <v>0</v>
+        <v>0.23</v>
       </c>
       <c r="G32">
-        <v>0.116182572614108</v>
+        <v>0.91277890466531397</v>
       </c>
       <c r="H32">
-        <v>0</v>
+        <v>0.91062039957939001</v>
       </c>
       <c r="I32">
-        <v>0.83099999999999996</v>
+        <v>0.80500000000000005</v>
       </c>
       <c r="J32">
-        <v>0.76900000000000002</v>
+        <v>0.622</v>
       </c>
       <c r="K32" t="s">
         <v>21</v>
@@ -8513,22 +8507,22 @@
         <v>21</v>
       </c>
       <c r="M32">
-        <v>0.89076923076923098</v>
+        <v>0.96</v>
       </c>
       <c r="N32">
-        <v>0.75438596491228105</v>
+        <v>0.94899999999999995</v>
       </c>
       <c r="O32">
-        <v>0.78286558345642498</v>
+        <v>0.94488188976377996</v>
       </c>
       <c r="P32">
-        <v>0.84884884884884904</v>
+        <v>0.960498960498961</v>
       </c>
       <c r="Q32">
-        <v>0.29099999999999998</v>
+        <v>0.89200000000000002</v>
       </c>
       <c r="R32">
-        <v>0.28000000000000003</v>
+        <v>0.81899999999999995</v>
       </c>
     </row>
     <row r="33" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
@@ -8536,7 +8530,7 @@
         <v>0.5</v>
       </c>
       <c r="B33">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C33" t="s">
         <v>1</v>
@@ -8545,22 +8539,22 @@
         <v>0</v>
       </c>
       <c r="E33">
-        <v>0.65</v>
+        <v>0.86199999999999999</v>
       </c>
       <c r="F33">
-        <v>0.02</v>
+        <v>0.221</v>
       </c>
       <c r="G33">
-        <v>0.75102459016393397</v>
+        <v>0.92008196721311497</v>
       </c>
       <c r="H33">
-        <v>0.77671232876712304</v>
+        <v>0.89669861554845598</v>
       </c>
       <c r="I33">
-        <v>0.78400000000000003</v>
+        <v>0.752</v>
       </c>
       <c r="J33">
-        <v>0.76700000000000002</v>
+        <v>0.51600000000000001</v>
       </c>
       <c r="K33" t="s">
         <v>21</v>
@@ -8569,27 +8563,27 @@
         <v>21</v>
       </c>
       <c r="M33">
-        <v>0.91725529767911196</v>
+        <v>0.91356783919597995</v>
       </c>
       <c r="N33">
-        <v>0.92400000000000004</v>
+        <v>0.72199999999999998</v>
       </c>
       <c r="O33">
-        <v>0.91666666666666696</v>
+        <v>0.93693693693693703</v>
       </c>
       <c r="P33">
-        <v>0.99198717948717996</v>
+        <v>0.94017094017094005</v>
       </c>
       <c r="Q33">
-        <v>0.84499999999999997</v>
+        <v>0.92700000000000005</v>
       </c>
       <c r="R33">
-        <v>0.59499999999999997</v>
+        <v>0.84199999999999997</v>
       </c>
     </row>
     <row r="34" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -8601,22 +8595,22 @@
         <v>0</v>
       </c>
       <c r="E34">
-        <v>0</v>
+        <v>0.85099999999999998</v>
       </c>
       <c r="F34">
-        <v>0</v>
+        <v>0.20399999999999999</v>
       </c>
       <c r="G34">
-        <v>1.14107883817427E-2</v>
+        <v>0.91402251791197497</v>
       </c>
       <c r="H34">
-        <v>0</v>
+        <v>0.90501043841336104</v>
       </c>
       <c r="I34">
-        <v>0.873</v>
+        <v>0.72899999999999998</v>
       </c>
       <c r="J34">
-        <v>0.54800000000000004</v>
+        <v>0.497</v>
       </c>
       <c r="K34" t="s">
         <v>21</v>
@@ -8625,22 +8619,22 @@
         <v>21</v>
       </c>
       <c r="M34">
-        <v>0.98404255319148903</v>
+        <v>0.89329268292682895</v>
       </c>
       <c r="N34">
-        <v>1</v>
+        <v>0.59199999999999997</v>
       </c>
       <c r="O34">
-        <v>0.96619718309859204</v>
+        <v>0.90769230769230802</v>
       </c>
       <c r="P34">
-        <v>0.88688688688688699</v>
+        <v>0.93069306930693096</v>
       </c>
       <c r="Q34">
-        <v>5.8000000000000003E-2</v>
+        <v>0.92400000000000004</v>
       </c>
       <c r="R34">
-        <v>0.26600000000000001</v>
+        <v>0.871</v>
       </c>
     </row>
     <row r="35" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
@@ -8648,87 +8642,87 @@
         <v>0.5</v>
       </c>
       <c r="B35">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="C35" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D35" t="s">
         <v>0</v>
       </c>
       <c r="E35">
-        <v>0.85099999999999998</v>
+        <v>0.54300000000000004</v>
       </c>
       <c r="F35">
-        <v>0.20399999999999999</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="G35">
-        <v>0.91402251791197497</v>
+        <v>0.69520897043832797</v>
       </c>
       <c r="H35">
-        <v>0.90501043841336104</v>
+        <v>0.66581956797967001</v>
       </c>
       <c r="I35">
-        <v>0.72899999999999998</v>
+        <v>0.79600000000000004</v>
       </c>
       <c r="J35">
+        <v>0.82499999999999996</v>
+      </c>
+      <c r="K35" t="s">
+        <v>21</v>
+      </c>
+      <c r="L35" t="s">
+        <v>21</v>
+      </c>
+      <c r="M35">
+        <v>0.83867735470941895</v>
+      </c>
+      <c r="N35">
         <v>0.497</v>
       </c>
-      <c r="K35" t="s">
-        <v>21</v>
-      </c>
-      <c r="L35" t="s">
-        <v>21</v>
-      </c>
-      <c r="M35">
-        <v>0.89329268292682895</v>
-      </c>
-      <c r="N35">
-        <v>0.59199999999999997</v>
-      </c>
       <c r="O35">
-        <v>0.90769230769230802</v>
+        <v>0.83689839572192504</v>
       </c>
       <c r="P35">
-        <v>0.93069306930693096</v>
+        <v>0.89716684155299098</v>
       </c>
       <c r="Q35">
-        <v>0.92400000000000004</v>
+        <v>0.79</v>
       </c>
       <c r="R35">
-        <v>0.871</v>
+        <v>0.40799999999999997</v>
       </c>
     </row>
     <row r="36" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="B36">
         <v>0.2</v>
       </c>
       <c r="C36" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D36" t="s">
         <v>0</v>
       </c>
       <c r="E36">
-        <v>0.01</v>
+        <v>0.65</v>
       </c>
       <c r="F36">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="G36">
-        <v>7.6053442959917797E-2</v>
+        <v>0.75102459016393397</v>
       </c>
       <c r="H36">
-        <v>0</v>
+        <v>0.77671232876712304</v>
       </c>
       <c r="I36">
-        <v>0.84099999999999997</v>
+        <v>0.78400000000000003</v>
       </c>
       <c r="J36">
-        <v>0.76600000000000001</v>
+        <v>0.76700000000000002</v>
       </c>
       <c r="K36" t="s">
         <v>21</v>
@@ -8737,22 +8731,22 @@
         <v>21</v>
       </c>
       <c r="M36">
-        <v>0.92084942084942101</v>
+        <v>0.91725529767911196</v>
       </c>
       <c r="N36">
-        <v>0.90756302521008403</v>
+        <v>0.92400000000000004</v>
       </c>
       <c r="O36">
-        <v>0.82196969696969702</v>
+        <v>0.91666666666666696</v>
       </c>
       <c r="P36">
-        <v>0.76161616161616197</v>
+        <v>0.99198717948717996</v>
       </c>
       <c r="Q36">
-        <v>0.29899999999999999</v>
+        <v>0.84499999999999997</v>
       </c>
       <c r="R36">
-        <v>0.28599999999999998</v>
+        <v>0.59499999999999997</v>
       </c>
     </row>
     <row r="37" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
@@ -8819,7 +8813,7 @@
       </filters>
     </filterColumn>
     <sortState ref="A14:R25">
-      <sortCondition ref="B1:B37"/>
+      <sortCondition ref="A1:A37"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>